<commit_message>
MongoDB connexion and FrontEnd inital commit
</commit_message>
<xml_diff>
--- a/Proyecto II - XTECDigital.xlsx
+++ b/Proyecto II - XTECDigital.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C310D9-08AF-4C24-9BDA-CACF7199893A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D9D487-5959-4E14-A7DF-6A607DA25E4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5805" yWindow="585" windowWidth="21570" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -436,6 +436,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -779,7 +785,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +956,7 @@
       <c r="A12" s="8">
         <v>8</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="18">
@@ -967,7 +973,7 @@
       <c r="A13" s="8">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="22" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="13">
@@ -984,7 +990,7 @@
       <c r="A14" s="8">
         <v>10</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="23" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="10">

</xml_diff>

<commit_message>
API Usuario SQL V2
</commit_message>
<xml_diff>
--- a/Proyecto II - XTECDigital.xlsx
+++ b/Proyecto II - XTECDigital.xlsx
@@ -1,26 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D9D487-5959-4E14-A7DF-6A607DA25E4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A137035-F3EB-422B-BDD6-D6DD15831E90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5805" yWindow="585" windowWidth="21570" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -462,7 +452,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -784,11 +774,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="53.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
@@ -830,7 +820,7 @@
       </c>
       <c r="D4" s="8">
         <f>SUM(D5:D61)</f>
-        <v>71.5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -946,7 +936,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>60</v>
@@ -1022,7 +1012,7 @@
         <v>0.5</v>
       </c>
       <c r="D16" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
         <v>61</v>
@@ -1039,7 +1029,7 @@
         <v>0.5</v>
       </c>
       <c r="D17" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
         <v>61</v>
@@ -1056,7 +1046,7 @@
         <v>0.5</v>
       </c>
       <c r="D18" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
         <v>61</v>
@@ -1073,7 +1063,7 @@
         <v>0.5</v>
       </c>
       <c r="D19" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>61</v>
@@ -1098,7 +1088,7 @@
         <v>0.5</v>
       </c>
       <c r="D21" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E21" t="s">
         <v>61</v>
@@ -1161,7 +1151,7 @@
         <v>0.5</v>
       </c>
       <c r="D26" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
         <v>61</v>
@@ -1178,7 +1168,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E27" t="s">
         <v>61</v>
@@ -1275,7 +1265,7 @@
         <v>0.5</v>
       </c>
       <c r="D35" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E35" t="s">
         <v>61</v>
@@ -1358,7 +1348,7 @@
         <v>0.5</v>
       </c>
       <c r="D42" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1372,7 +1362,7 @@
         <v>0.5</v>
       </c>
       <c r="D43" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1386,7 +1376,7 @@
         <v>0.5</v>
       </c>
       <c r="D44" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1400,7 +1390,7 @@
         <v>4.5</v>
       </c>
       <c r="D45" s="10">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E45" s="21"/>
     </row>

</xml_diff>